<commit_message>
update new files example for insumos and reportes
</commit_message>
<xml_diff>
--- a/app/Reportes/Devolucion_Ventas.xlsx
+++ b/app/Reportes/Devolucion_Ventas.xlsx
@@ -501,10 +501,22 @@
           <t>901097122</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CALLE 10A NO. 1 - 21 SUR, FACA </t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>3174325821</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>carnesfaca.10@gmail.com</t>
+        </is>
+      </c>
       <c r="G2" t="n">
         <v>14201.68</v>
       </c>
@@ -533,9 +545,19 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">VEREDA CHIGUALA, VILLAPINZÓN </t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>3112764625</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>jhon.cartertorres@gmail.com</t>
+        </is>
+      </c>
       <c r="G3" t="n">
         <v>553865.53</v>
       </c>

</xml_diff>